<commit_message>
get index row by account total
</commit_message>
<xml_diff>
--- a/src/Opex.xlsx
+++ b/src/Opex.xlsx
@@ -295,170 +295,6 @@
     </indexedColors>
   </colors>
 </styleSheet>
-</file>
-
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
-  <style val="10"/>
-  <chart>
-    <title>
-      <tx>
-        <rich>
-          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:t>Bar Chart</a:t>
-            </a:r>
-          </a:p>
-        </rich>
-      </tx>
-    </title>
-    <plotArea>
-      <barChart>
-        <barDir val="col"/>
-        <grouping val="clustered"/>
-        <ser>
-          <idx val="0"/>
-          <order val="0"/>
-          <tx>
-            <strRef>
-              <f>'Relatório'!B1</f>
-            </strRef>
-          </tx>
-          <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <cat>
-            <numRef>
-              <f>'Relatório'!$A$2:$A$7</f>
-            </numRef>
-          </cat>
-          <val>
-            <numRef>
-              <f>'Relatório'!$B$2:$B$7</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="1"/>
-          <order val="1"/>
-          <tx>
-            <strRef>
-              <f>'Relatório'!C1</f>
-            </strRef>
-          </tx>
-          <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <cat>
-            <numRef>
-              <f>'Relatório'!$A$2:$A$7</f>
-            </numRef>
-          </cat>
-          <val>
-            <numRef>
-              <f>'Relatório'!$C$2:$C$7</f>
-            </numRef>
-          </val>
-        </ser>
-        <gapWidth val="150"/>
-        <axId val="10"/>
-        <axId val="100"/>
-      </barChart>
-      <catAx>
-        <axId val="10"/>
-        <scaling>
-          <orientation val="minMax"/>
-        </scaling>
-        <axPos val="l"/>
-        <title>
-          <tx>
-            <rich>
-              <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-              <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:t>Sample length (mm)</a:t>
-                </a:r>
-              </a:p>
-            </rich>
-          </tx>
-        </title>
-        <majorTickMark val="none"/>
-        <minorTickMark val="none"/>
-        <crossAx val="100"/>
-        <lblOffset val="100"/>
-      </catAx>
-      <valAx>
-        <axId val="100"/>
-        <scaling>
-          <orientation val="minMax"/>
-        </scaling>
-        <axPos val="l"/>
-        <majorGridlines/>
-        <title>
-          <tx>
-            <rich>
-              <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-              <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:t>Test number</a:t>
-                </a:r>
-              </a:p>
-            </rich>
-          </tx>
-        </title>
-        <majorTickMark val="none"/>
-        <minorTickMark val="none"/>
-        <crossAx val="10"/>
-      </valAx>
-    </plotArea>
-    <legend>
-      <legendPos val="r"/>
-    </legend>
-    <plotVisOnly val="1"/>
-    <dispBlanksAs val="gap"/>
-  </chart>
-</chartSpace>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
-  <oneCellAnchor>
-    <from>
-      <col>0</col>
-      <colOff>0</colOff>
-      <row>9</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="5400000" cy="2700000"/>
-    <graphicFrame>
-      <nvGraphicFramePr>
-        <cNvPr id="1" name="Chart 1"/>
-        <cNvGraphicFramePr/>
-      </nvGraphicFramePr>
-      <xfrm/>
-      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </graphicFrame>
-    <clientData/>
-  </oneCellAnchor>
-</wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1764,7 +1600,9 @@
         <v>1503</v>
       </c>
       <c r="P20" s="11" t="n"/>
-      <c r="Q20" s="11" t="n"/>
+      <c r="Q20" s="11" t="n">
+        <v>27979.15</v>
+      </c>
       <c r="R20" s="11" t="n"/>
       <c r="S20" s="12" t="n">
         <v>-19077.77</v>
@@ -3266,8 +3104,12 @@
       <c r="P50" s="13" t="n">
         <v>1950.7778</v>
       </c>
-      <c r="Q50" s="13" t="n"/>
-      <c r="R50" s="13" t="n"/>
+      <c r="Q50" s="13" t="n">
+        <v>1604.61</v>
+      </c>
+      <c r="R50" s="13" t="n">
+        <v>346.1677999999997</v>
+      </c>
       <c r="S50" s="13" t="n">
         <v>346.1999999999998</v>
       </c>
@@ -6159,6 +6001,5 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>